<commit_message>
Clean up and re-org
</commit_message>
<xml_diff>
--- a/docs/assets/references/frame/FrameCalculator.xlsx
+++ b/docs/assets/references/frame/FrameCalculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8bf86f88c49aa82/Documents/GitHub/HevORT/docs/assets/references/frame/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{0DFE4DA3-9321-4DE1-8882-F27B64FDD3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBB8B9C3-1348-48CD-A1F8-CF11481C8CE2}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{0DFE4DA3-9321-4DE1-8882-F27B64FDD3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83F77046-2B5F-4036-9613-9DF249554A84}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{2DD4E541-7648-4A97-AB5A-A9C0E0660C31}"/>
   </bookViews>
@@ -2869,7 +2869,7 @@
   </sheetPr>
   <dimension ref="A1:W55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -2912,7 +2912,7 @@
         <v>2</v>
       </c>
       <c r="H2" s="5">
-        <v>415</v>
+        <v>315</v>
       </c>
       <c r="I2" s="17" t="s">
         <v>105</v>
@@ -2925,7 +2925,7 @@
       </c>
       <c r="H3" s="6">
         <f>H2</f>
-        <v>415</v>
+        <v>315</v>
       </c>
       <c r="I3" t="s">
         <v>4</v>
@@ -2973,7 +2973,7 @@
       </c>
       <c r="Q6" s="56" t="str">
         <f>"Summary for: "&amp;H2&amp;"x"&amp;H3&amp;"x"&amp;H4&amp;" - "&amp;H5</f>
-        <v>Summary for: 415x415x340 - HD</v>
+        <v>Summary for: 315x315x340 - HD</v>
       </c>
       <c r="R6" s="57"/>
       <c r="S6" s="58"/>
@@ -3051,7 +3051,7 @@
       </c>
       <c r="I8" s="14">
         <f t="shared" ref="I8:I52" si="1">IFERROR(VLOOKUP(K8,$G$2:$H$4,2,0),0)+M8</f>
-        <v>520</v>
+        <v>420</v>
       </c>
       <c r="J8" s="14">
         <v>1</v>
@@ -3100,7 +3100,7 @@
       </c>
       <c r="I9" s="14">
         <f t="shared" si="1"/>
-        <v>520</v>
+        <v>420</v>
       </c>
       <c r="J9" s="14">
         <v>1</v>
@@ -3149,7 +3149,7 @@
       </c>
       <c r="I10" s="14">
         <f t="shared" si="1"/>
-        <v>510</v>
+        <v>410</v>
       </c>
       <c r="J10" s="14">
         <v>1</v>
@@ -3198,7 +3198,7 @@
       </c>
       <c r="I11" s="14">
         <f t="shared" si="1"/>
-        <v>510</v>
+        <v>410</v>
       </c>
       <c r="J11" s="14">
         <v>1</v>
@@ -3241,7 +3241,7 @@
       </c>
       <c r="I12" s="14">
         <f t="shared" si="1"/>
-        <v>520</v>
+        <v>420</v>
       </c>
       <c r="J12" s="14">
         <v>1</v>
@@ -3290,7 +3290,7 @@
       </c>
       <c r="I13" s="14">
         <f t="shared" si="1"/>
-        <v>520</v>
+        <v>420</v>
       </c>
       <c r="J13" s="14">
         <v>1</v>
@@ -3339,7 +3339,7 @@
       </c>
       <c r="I14" s="14">
         <f t="shared" si="1"/>
-        <v>510</v>
+        <v>410</v>
       </c>
       <c r="J14" s="14">
         <v>1</v>
@@ -3388,7 +3388,7 @@
       </c>
       <c r="I15" s="14">
         <f t="shared" si="1"/>
-        <v>510</v>
+        <v>410</v>
       </c>
       <c r="J15" s="14">
         <v>1</v>
@@ -3437,7 +3437,7 @@
       </c>
       <c r="I16" s="14">
         <f t="shared" si="1"/>
-        <v>520</v>
+        <v>420</v>
       </c>
       <c r="J16" s="14">
         <v>1</v>
@@ -3486,7 +3486,7 @@
       </c>
       <c r="I17" s="14">
         <f t="shared" si="1"/>
-        <v>510</v>
+        <v>410</v>
       </c>
       <c r="J17" s="14">
         <v>1</v>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="I18" s="14">
         <f t="shared" si="1"/>
-        <v>510</v>
+        <v>410</v>
       </c>
       <c r="J18" s="14">
         <v>1</v>
@@ -3768,7 +3768,7 @@
       </c>
       <c r="I23" s="14">
         <f t="shared" si="1"/>
-        <v>510</v>
+        <v>410</v>
       </c>
       <c r="J23" s="14">
         <v>1</v>
@@ -4001,7 +4001,7 @@
       </c>
       <c r="I28" s="14">
         <f t="shared" si="1"/>
-        <v>510</v>
+        <v>410</v>
       </c>
       <c r="J28" s="14">
         <v>1</v>
@@ -4272,7 +4272,7 @@
       </c>
       <c r="I34" s="14">
         <f t="shared" si="1"/>
-        <v>360</v>
+        <v>260</v>
       </c>
       <c r="J34" s="14">
         <v>1</v>
@@ -4315,7 +4315,7 @@
       </c>
       <c r="I35" s="14">
         <f t="shared" si="1"/>
-        <v>360</v>
+        <v>260</v>
       </c>
       <c r="J35" s="14">
         <v>1</v>
@@ -4358,7 +4358,7 @@
       </c>
       <c r="I36" s="14">
         <f t="shared" si="1"/>
-        <v>420</v>
+        <v>320</v>
       </c>
       <c r="J36" s="14">
         <v>1</v>
@@ -4401,7 +4401,7 @@
       </c>
       <c r="I37" s="14">
         <f t="shared" si="1"/>
-        <v>420</v>
+        <v>320</v>
       </c>
       <c r="J37" s="14">
         <v>1</v>
@@ -4441,7 +4441,7 @@
       </c>
       <c r="I38" s="14">
         <f t="shared" si="1"/>
-        <v>531</v>
+        <v>431</v>
       </c>
       <c r="J38" s="14">
         <v>1</v>
@@ -4489,7 +4489,7 @@
       </c>
       <c r="I39" s="14">
         <f t="shared" si="1"/>
-        <v>440</v>
+        <v>340</v>
       </c>
       <c r="J39" s="14">
         <v>1</v>
@@ -4533,7 +4533,7 @@
       </c>
       <c r="I40" s="14">
         <f t="shared" si="1"/>
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J40" s="14">
         <v>1</v>
@@ -4577,7 +4577,7 @@
       </c>
       <c r="I41" s="14">
         <f t="shared" si="1"/>
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J41" s="14">
         <v>1</v>
@@ -4623,7 +4623,7 @@
       </c>
       <c r="I42" s="14">
         <f t="shared" si="1"/>
-        <v>485</v>
+        <v>385</v>
       </c>
       <c r="J42" s="14">
         <v>1</v>
@@ -4997,7 +4997,7 @@
       </c>
       <c r="I50" s="14">
         <f>IFERROR(VLOOKUP(K50,$G$2:$H$4,2,0)*8,0)+M50</f>
-        <v>4800</v>
+        <v>4000</v>
       </c>
       <c r="J50" s="14">
         <v>1</v>
@@ -5037,7 +5037,7 @@
       </c>
       <c r="I51" s="14">
         <f t="shared" si="1"/>
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="J51" s="14">
         <v>1</v>
@@ -5075,7 +5075,7 @@
       </c>
       <c r="I52" s="14">
         <f t="shared" si="1"/>
-        <v>520</v>
+        <v>420</v>
       </c>
       <c r="J52" s="14">
         <v>1</v>
@@ -5113,7 +5113,7 @@
       </c>
       <c r="I53" s="14">
         <f t="shared" ref="I53:I55" si="4">IFERROR(VLOOKUP(K53,$G$2:$H$4,2,0),0)+M53</f>
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J53" s="14">
         <v>1</v>
@@ -5152,7 +5152,7 @@
       </c>
       <c r="I54" s="14">
         <f t="shared" si="4"/>
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J54" s="14">
         <v>1</v>
@@ -5191,7 +5191,7 @@
       </c>
       <c r="I55" s="14">
         <f t="shared" si="4"/>
-        <v>450</v>
+        <v>350</v>
       </c>
       <c r="J55" s="14">
         <v>1</v>
@@ -5226,7 +5226,7 @@
       <formula>$D8&lt;&gt;"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5" xr:uid="{43ABBEE6-5061-4C4F-BA60-D00D88D865EC}">
       <formula1>"STD_HT, HD"</formula1>
     </dataValidation>
@@ -5277,7 +5277,7 @@
       </c>
       <c r="Q5" s="45">
         <f>FRAMECALCULATOR!H2</f>
-        <v>415</v>
+        <v>315</v>
       </c>
     </row>
     <row r="6" spans="16:17" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
@@ -5287,7 +5287,7 @@
       </c>
       <c r="Q6" s="47">
         <f>FRAMECALCULATOR!H3</f>
-        <v>415</v>
+        <v>315</v>
       </c>
     </row>
     <row r="9" spans="16:17" ht="15.5" x14ac:dyDescent="0.35">
@@ -5304,7 +5304,7 @@
       </c>
       <c r="Q10" s="39">
         <f>Q5+25</f>
-        <v>440</v>
+        <v>340</v>
       </c>
     </row>
     <row r="11" spans="16:17" ht="21" x14ac:dyDescent="0.5">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="Q11" s="39">
         <f>Q6+25</f>
-        <v>440</v>
+        <v>340</v>
       </c>
     </row>
     <row r="13" spans="16:17" ht="15.5" x14ac:dyDescent="0.35">
@@ -5330,7 +5330,7 @@
       </c>
       <c r="Q14" s="39">
         <f>Q5+12</f>
-        <v>427</v>
+        <v>327</v>
       </c>
     </row>
     <row r="15" spans="16:17" ht="21" x14ac:dyDescent="0.5">
@@ -5339,7 +5339,7 @@
       </c>
       <c r="Q15" s="39">
         <f>Q6+-13</f>
-        <v>402</v>
+        <v>302</v>
       </c>
     </row>
     <row r="17" spans="16:17" ht="15.5" x14ac:dyDescent="0.35">
@@ -5354,7 +5354,7 @@
       </c>
       <c r="Q18" s="39">
         <f>Q5-15</f>
-        <v>400</v>
+        <v>300</v>
       </c>
     </row>
     <row r="19" spans="16:17" ht="21" x14ac:dyDescent="0.5">
@@ -5363,7 +5363,7 @@
       </c>
       <c r="Q19" s="39">
         <f>Q6-15</f>
-        <v>400</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>